<commit_message>
Updated as of 29-11-2017
</commit_message>
<xml_diff>
--- a/Workspace/AutomatedTestingWeek/properties.xlsx
+++ b/Workspace/AutomatedTestingWeek/properties.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -45,6 +45,18 @@
   </si>
   <si>
     <t>1234</t>
+  </si>
+  <si>
+    <t>demoQAHomepage</t>
+  </si>
+  <si>
+    <t>http://www.demoqa.com/</t>
+  </si>
+  <si>
+    <t>MoveAmountY</t>
+  </si>
+  <si>
+    <t>MoveAmountX</t>
   </si>
 </sst>
 </file>
@@ -89,10 +101,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -374,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,11 +432,36 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated as of 30/11/2017
</commit_message>
<xml_diff>
--- a/Workspace/AutomatedTestingWeek/properties.xlsx
+++ b/Workspace/AutomatedTestingWeek/properties.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12885" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
+    <sheet name="persons" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
   <si>
     <t>username</t>
   </si>
@@ -57,6 +58,129 @@
   </si>
   <si>
     <t>MoveAmountX</t>
+  </si>
+  <si>
+    <t>DriverSelector</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>Store Home Page</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Owen</t>
+  </si>
+  <si>
+    <t>website details</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>owen</t>
+  </si>
+  <si>
+    <t>chapman</t>
+  </si>
+  <si>
+    <t>test123@haha.lul</t>
+  </si>
+  <si>
+    <t>drowssap</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>AddressLine One</t>
+  </si>
+  <si>
+    <t>In This Town</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>This isnt a real address you fool!</t>
+  </si>
+  <si>
+    <t>AliasAddressONE</t>
+  </si>
+  <si>
+    <t>07865772243</t>
+  </si>
+  <si>
+    <t>01944888765</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Address Line One</t>
+  </si>
+  <si>
+    <t>Address Line Two</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>ZIP</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Additional Info</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alias </t>
+  </si>
+  <si>
+    <t>Chapman</t>
+  </si>
+  <si>
+    <t>test123@qa.com</t>
+  </si>
+  <si>
+    <t>8/12/1994</t>
   </si>
 </sst>
 </file>
@@ -101,12 +225,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -388,19 +513,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,7 +549,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -416,7 +557,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -424,7 +565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -432,7 +573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -440,7 +581,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -448,20 +589,291 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="4">
         <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" t="s">
+        <v>44</v>
+      </c>
+      <c r="O10" t="s">
+        <v>45</v>
+      </c>
+      <c r="P10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>47</v>
+      </c>
+      <c r="R10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="5">
+        <v>34676</v>
+      </c>
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11">
+        <v>63909</v>
+      </c>
+      <c r="N11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R11" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="E11" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2">
+        <v>63909</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>